<commit_message>
Add database schema and data sample.
</commit_message>
<xml_diff>
--- a/Schema_Data/Data.xlsx
+++ b/Schema_Data/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Year3\HK2\PTTK\Project\Schema_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A88FB2-8D27-49C0-8097-647F7425AC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4CBFA5-C017-438D-8528-7E65A5438620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{A9C2B380-941E-4AF3-AF89-697926482C6B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="10" activeTab="15" xr2:uid="{A9C2B380-941E-4AF3-AF89-697926482C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="UNGVIEN" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,16 @@
     <sheet name="HINHTHUC" sheetId="4" r:id="rId4"/>
     <sheet name="CAPBAC" sheetId="5" r:id="rId5"/>
     <sheet name="VITRI" sheetId="6" r:id="rId6"/>
-    <sheet name="HOPDONG" sheetId="7" r:id="rId7"/>
-    <sheet name="HINHTHUC_HOPDONG" sheetId="8" r:id="rId8"/>
-    <sheet name="HOADON" sheetId="9" r:id="rId9"/>
-    <sheet name="UUDAI" sheetId="10" r:id="rId10"/>
-    <sheet name="HSUNGTUYEN" sheetId="11" r:id="rId11"/>
-    <sheet name="GIAYTOUV" sheetId="12" r:id="rId12"/>
-    <sheet name="NVPHANHOI" sheetId="13" r:id="rId13"/>
-    <sheet name="DNPHANHOI" sheetId="14" r:id="rId14"/>
+    <sheet name="KYNANG" sheetId="15" r:id="rId7"/>
+    <sheet name="HOPDONG" sheetId="7" r:id="rId8"/>
+    <sheet name="HINHTHUC_HOPDONG" sheetId="8" r:id="rId9"/>
+    <sheet name="HOPDONG_KYNANG" sheetId="16" r:id="rId10"/>
+    <sheet name="HOADON" sheetId="9" r:id="rId11"/>
+    <sheet name="UUDAI" sheetId="10" r:id="rId12"/>
+    <sheet name="HSUNGTUYEN" sheetId="11" r:id="rId13"/>
+    <sheet name="GIAYTOUV" sheetId="12" r:id="rId14"/>
+    <sheet name="NVPHANHOI" sheetId="13" r:id="rId15"/>
+    <sheet name="DNPHANHOI" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,10 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
-  <si>
-    <t xml:space="preserve"> MAUV</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="228">
   <si>
     <t>HOTEN</t>
   </si>
@@ -270,9 +269,6 @@
     <t>NV00000005</t>
   </si>
   <si>
-    <t>Nhân viên</t>
-  </si>
-  <si>
     <t>NV00000006</t>
   </si>
   <si>
@@ -288,9 +284,6 @@
     <t>NV00000010</t>
   </si>
   <si>
-    <t>Ban lãnh đạo</t>
-  </si>
-  <si>
     <t>DN00000001</t>
   </si>
   <si>
@@ -342,9 +335,6 @@
     <t>GIAYBAO</t>
   </si>
   <si>
-    <t>MANGXH</t>
-  </si>
-  <si>
     <t>Tuyển dụng trên mạng xã hội</t>
   </si>
   <si>
@@ -400,15 +390,357 @@
   </si>
   <si>
     <t>All Levels</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Product Manager</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>System Admin</t>
+  </si>
+  <si>
+    <t>System Engineer</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Data Engineer</t>
+  </si>
+  <si>
+    <t>Full-stack</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Front-end Developer</t>
+  </si>
+  <si>
+    <t>Back-end Developer</t>
+  </si>
+  <si>
+    <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Security Engineer</t>
+  </si>
+  <si>
+    <t>Security Developer</t>
+  </si>
+  <si>
+    <t>Security Architect</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>FE</t>
+  </si>
+  <si>
+    <t>SCRUM</t>
+  </si>
+  <si>
+    <t>SCA</t>
+  </si>
+  <si>
+    <t>SCD</t>
+  </si>
+  <si>
+    <t>SCE</t>
+  </si>
+  <si>
+    <t>SYSE</t>
+  </si>
+  <si>
+    <t>QC</t>
+  </si>
+  <si>
+    <t>MAKN</t>
+  </si>
+  <si>
+    <t>JavaScript</t>
+  </si>
+  <si>
+    <t>Flutter</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>Java</t>
+  </si>
+  <si>
+    <t>.NET</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>iOS</t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>DevOps</t>
+  </si>
+  <si>
+    <t>Golang</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>Cloud</t>
+  </si>
+  <si>
+    <t>UI/UX</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>Unity</t>
+  </si>
+  <si>
+    <t>Kotlin</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>NodeJS</t>
+  </si>
+  <si>
+    <t>ReactJS</t>
+  </si>
+  <si>
+    <t>VueJS</t>
+  </si>
+  <si>
+    <t>Laravel</t>
+  </si>
+  <si>
+    <t>ASP.NET</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>AngularJS</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Embedded</t>
+  </si>
+  <si>
+    <t>React</t>
+  </si>
+  <si>
+    <t>HD00000001</t>
+  </si>
+  <si>
+    <t>HD00000002</t>
+  </si>
+  <si>
+    <t>HD00000003</t>
+  </si>
+  <si>
+    <t>HD00000004</t>
+  </si>
+  <si>
+    <t>HD00000005</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang tìm kiếm một intern back-end năng động và ham học hỏi để tham gia vào đội ngũ phát triển phần mềm của chúng tôi. Ứng viên lý tưởng sẽ có kiến thức cơ bản về lập trình back-end và mong muốn học hỏi và phát triển kỹ năng trong môi trường làm việc thực tế.</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang tìm kiếm một fresher business analyst đam mê và sáng tạo để tham gia vào đội ngũ phân tích kinh doanh của chúng tôi. Ứng viên lý tưởng sẽ có kiến thức cơ bản về phân tích kinh doanh và khả năng làm việc trong môi trường đa dạng và động.</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang tìm kiếm một junior data analyst nhiệt huyết và có kỹ năng phân tích dữ liệu để tham gia vào đội ngũ phân tích dữ liệu của chúng tôi. Ứng viên lý tưởng sẽ có kiến thức cơ bản về phân tích dữ liệu và mong muốn phát triển kỹ năng trong lĩnh vực này.</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang tìm kiếm một middle developer có kinh nghiệm và sáng tạo để tham gia vào đội ngũ phát triển phần mềm của chúng tôi. Ứng viên lý tưởng sẽ có kinh nghiệm trong việc phát triển phần mềm, kiến thức vững về các ngôn ngữ lập trình và có khả năng làm việc hiệu quả trong môi trường đội nhóm.</t>
+  </si>
+  <si>
+    <t>Chúng tôi đang tìm kiếm một senior developer có kinh nghiệm và năng động để tham gia vào đội ngũ phát triển phần mềm của chúng tôi và đóng góp vào việc xây dựng các sản phẩm chất lượng. Ứng viên lý tưởng sẽ có kinh nghiệm rộng lớn trong việc phát triển phần mềm, lãnh đạo và hướng dẫn các thành viên khác trong đội ngũ.</t>
+  </si>
+  <si>
+    <t>MXH</t>
+  </si>
+  <si>
+    <t>ANDROID</t>
+  </si>
+  <si>
+    <t>ANGULAR</t>
+  </si>
+  <si>
+    <t>ANGULARJS</t>
+  </si>
+  <si>
+    <t>AZURE</t>
+  </si>
+  <si>
+    <t>CLOUD</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
+  <si>
+    <t>DEVOPS</t>
+  </si>
+  <si>
+    <t>EMBEDDED</t>
+  </si>
+  <si>
+    <t>FLUTTER</t>
+  </si>
+  <si>
+    <t>GAME</t>
+  </si>
+  <si>
+    <t>GOLANG</t>
+  </si>
+  <si>
+    <t>IOS</t>
+  </si>
+  <si>
+    <t>JAVA</t>
+  </si>
+  <si>
+    <t>JAVASCRIPT</t>
+  </si>
+  <si>
+    <t>KOTLIN</t>
+  </si>
+  <si>
+    <t>LARAVEL</t>
+  </si>
+  <si>
+    <t>MOBILE</t>
+  </si>
+  <si>
+    <t>NETWORK</t>
+  </si>
+  <si>
+    <t>NODEJS</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
+  </si>
+  <si>
+    <t>REACT</t>
+  </si>
+  <si>
+    <t>REACTJS</t>
+  </si>
+  <si>
+    <t>TESTER</t>
+  </si>
+  <si>
+    <t>UNITY</t>
+  </si>
+  <si>
+    <t>VUEJS</t>
+  </si>
+  <si>
+    <t>NGAYLAP</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>Thẻ</t>
+  </si>
+  <si>
+    <t>Giới thiệu 1</t>
+  </si>
+  <si>
+    <t>Giới thiệu 2</t>
+  </si>
+  <si>
+    <t>Giới thiệu 3</t>
+  </si>
+  <si>
+    <t>Giới thiệu 4</t>
+  </si>
+  <si>
+    <t>Giới thiệu 5</t>
+  </si>
+  <si>
+    <t>HCMUS</t>
+  </si>
+  <si>
+    <t>3 Năm kinh nghiệm C++</t>
+  </si>
+  <si>
+    <t>IELTS</t>
+  </si>
+  <si>
+    <t>Overall 9.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -463,10 +795,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -805,7 +1137,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G2:G6"/>
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,140 +1152,140 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2">
+        <v>54</v>
+      </c>
+      <c r="D2" s="5">
         <v>37622</v>
       </c>
       <c r="E2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>63</v>
+      <c r="G2" s="2" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="2">
+        <v>54</v>
+      </c>
+      <c r="D3" s="5">
         <v>37623</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="2">
+        <v>54</v>
+      </c>
+      <c r="D4" s="5">
         <v>37624</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="2">
+        <v>54</v>
+      </c>
+      <c r="D5" s="5">
         <v>37625</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="5">
+        <v>37626</v>
+      </c>
+      <c r="E6" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="2">
-        <v>37626</v>
-      </c>
-      <c r="E6" t="s">
-        <v>57</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -971,91 +1303,400 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F958F3D-8A31-4430-808E-13FDB399CAA3}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E6525D-D9C1-4647-BC0F-412D3A528147}">
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>184</v>
+      </c>
+      <c r="B22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C33C99-5584-4992-A1AF-353F41404BC4}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF1C386-722F-4295-863A-69DD06659867}">
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7265625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="5">
+        <v>45395</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="5">
+        <v>45396</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" s="5">
+        <v>45397</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45398</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" s="5">
+        <v>45399</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>217</v>
+      </c>
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D276222B-0DF3-498C-9C12-37599D31CC57}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F958F3D-8A31-4430-808E-13FDB399CAA3}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1064,6 +1705,1013 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6C33C99-5584-4992-A1AF-353F41404BC4}">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="5">
+        <v>45402</v>
+      </c>
+      <c r="D2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="5">
+        <v>45402</v>
+      </c>
+      <c r="D3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="5">
+        <v>45402</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="5">
+        <v>45402</v>
+      </c>
+      <c r="D5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E5" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="5">
+        <v>45402</v>
+      </c>
+      <c r="D6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" t="s">
+        <v>224</v>
+      </c>
+      <c r="F6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" s="5">
+        <v>45403</v>
+      </c>
+      <c r="D7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" s="5">
+        <v>45403</v>
+      </c>
+      <c r="D8" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" t="s">
+        <v>224</v>
+      </c>
+      <c r="F8" t="s">
+        <v>225</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" s="5">
+        <v>45403</v>
+      </c>
+      <c r="D9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E9" t="s">
+        <v>224</v>
+      </c>
+      <c r="F9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" s="5">
+        <v>45403</v>
+      </c>
+      <c r="D10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F10" t="s">
+        <v>225</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45403</v>
+      </c>
+      <c r="D11" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" t="s">
+        <v>225</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45404</v>
+      </c>
+      <c r="D12" t="s">
+        <v>219</v>
+      </c>
+      <c r="E12" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" t="s">
+        <v>225</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="5">
+        <v>45404</v>
+      </c>
+      <c r="D13" t="s">
+        <v>220</v>
+      </c>
+      <c r="E13" t="s">
+        <v>224</v>
+      </c>
+      <c r="F13" t="s">
+        <v>225</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45404</v>
+      </c>
+      <c r="D14" t="s">
+        <v>221</v>
+      </c>
+      <c r="E14" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" t="s">
+        <v>225</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45404</v>
+      </c>
+      <c r="D15" t="s">
+        <v>222</v>
+      </c>
+      <c r="E15" t="s">
+        <v>224</v>
+      </c>
+      <c r="F15" t="s">
+        <v>225</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="5">
+        <v>45404</v>
+      </c>
+      <c r="D16" t="s">
+        <v>223</v>
+      </c>
+      <c r="E16" t="s">
+        <v>224</v>
+      </c>
+      <c r="F16" t="s">
+        <v>225</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="5">
+        <v>45405</v>
+      </c>
+      <c r="D17" t="s">
+        <v>219</v>
+      </c>
+      <c r="E17" t="s">
+        <v>224</v>
+      </c>
+      <c r="F17" t="s">
+        <v>225</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="5">
+        <v>45405</v>
+      </c>
+      <c r="D18" t="s">
+        <v>220</v>
+      </c>
+      <c r="E18" t="s">
+        <v>224</v>
+      </c>
+      <c r="F18" t="s">
+        <v>225</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="5">
+        <v>45405</v>
+      </c>
+      <c r="D19" t="s">
+        <v>221</v>
+      </c>
+      <c r="E19" t="s">
+        <v>224</v>
+      </c>
+      <c r="F19" t="s">
+        <v>225</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="5">
+        <v>45405</v>
+      </c>
+      <c r="D20" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" t="s">
+        <v>225</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="5">
+        <v>45405</v>
+      </c>
+      <c r="D21" t="s">
+        <v>223</v>
+      </c>
+      <c r="E21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F21" t="s">
+        <v>225</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" s="5">
+        <v>45406</v>
+      </c>
+      <c r="D22" t="s">
+        <v>219</v>
+      </c>
+      <c r="E22" t="s">
+        <v>224</v>
+      </c>
+      <c r="F22" t="s">
+        <v>225</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C23" s="5">
+        <v>45406</v>
+      </c>
+      <c r="D23" t="s">
+        <v>220</v>
+      </c>
+      <c r="E23" t="s">
+        <v>224</v>
+      </c>
+      <c r="F23" t="s">
+        <v>225</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" s="5">
+        <v>45406</v>
+      </c>
+      <c r="D24" t="s">
+        <v>221</v>
+      </c>
+      <c r="E24" t="s">
+        <v>224</v>
+      </c>
+      <c r="F24" t="s">
+        <v>225</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" s="5">
+        <v>45406</v>
+      </c>
+      <c r="D25" t="s">
+        <v>222</v>
+      </c>
+      <c r="E25" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" t="s">
+        <v>225</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" s="5">
+        <v>45406</v>
+      </c>
+      <c r="D26" t="s">
+        <v>223</v>
+      </c>
+      <c r="E26" t="s">
+        <v>224</v>
+      </c>
+      <c r="F26" t="s">
+        <v>225</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D276222B-0DF3-498C-9C12-37599D31CC57}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C7" t="s">
+        <v>226</v>
+      </c>
+      <c r="D7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D8" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C10" t="s">
+        <v>226</v>
+      </c>
+      <c r="D10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" t="s">
+        <v>226</v>
+      </c>
+      <c r="D13" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" t="s">
+        <v>226</v>
+      </c>
+      <c r="D14" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" t="s">
+        <v>226</v>
+      </c>
+      <c r="D17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" t="s">
+        <v>226</v>
+      </c>
+      <c r="D19" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" t="s">
+        <v>226</v>
+      </c>
+      <c r="D20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" t="s">
+        <v>226</v>
+      </c>
+      <c r="D21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>184</v>
+      </c>
+      <c r="C22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C23" t="s">
+        <v>226</v>
+      </c>
+      <c r="D23" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>184</v>
+      </c>
+      <c r="C24" t="s">
+        <v>226</v>
+      </c>
+      <c r="D24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" t="s">
+        <v>227</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF277982-4EBE-4FCA-ABF6-7FB774C7B7B1}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -1075,16 +2723,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1092,25 +2740,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB20A08-185D-48E3-8DB2-CDE84B0FEB50}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +2771,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1135,123 +2783,123 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
+        <v>49</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" t="s">
-        <v>73</v>
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>73</v>
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>73</v>
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" t="s">
-        <v>79</v>
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>79</v>
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>79</v>
+        <v>53</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1265,7 +2913,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,147 +2924,164 @@
     <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>1111111111</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>63</v>
+        <v>87</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>2222222222</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>64</v>
+        <v>88</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>3333333333</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>65</v>
+        <v>89</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>4444444444</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>66</v>
+        <v>90</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6">
         <v>5555555555</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>67</v>
+        <v>91</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1438,7 +3103,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,45 +3114,45 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="4">
+        <v>95</v>
+      </c>
+      <c r="C2" s="3">
         <v>100000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C3" s="4">
+        <v>96</v>
+      </c>
+      <c r="C3" s="3">
         <v>200000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>190</v>
       </c>
       <c r="B4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="4">
+        <v>94</v>
+      </c>
+      <c r="C4" s="3">
         <v>300000</v>
       </c>
     </row>
@@ -1501,7 +3166,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,100 +3178,100 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="C6" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="4">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="C7" s="3">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="4">
-        <v>300000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C8" s="3">
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="4">
-        <v>400000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C6" s="4">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C7" s="4">
-        <v>600000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" s="4">
-        <v>700000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>800000</v>
       </c>
     </row>
@@ -1617,131 +3282,958 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E606A4-599A-4316-B59C-EA7C97527E36}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>16</v>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+      <c r="C13" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C14" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>137</v>
+      </c>
+      <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>145</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="3">
+        <v>400000</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C18">
+    <sortCondition ref="B2:B18"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52412B7-2386-4655-B84B-EEB748633C00}">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D07F50D-1B3C-4D08-A166-F7398178BD09}">
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C7" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C8" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>155</v>
+      </c>
+      <c r="B10" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" t="s">
+        <v>178</v>
+      </c>
+      <c r="C14" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>199</v>
+      </c>
+      <c r="B15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>200</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>202</v>
+      </c>
+      <c r="B19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C19" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B20" t="s">
+        <v>150</v>
+      </c>
+      <c r="C20" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>204</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>205</v>
+      </c>
+      <c r="B22" t="s">
+        <v>167</v>
+      </c>
+      <c r="C22" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C24" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25" s="3">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="3">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>210</v>
+      </c>
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>211</v>
+      </c>
+      <c r="B29" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>212</v>
+      </c>
+      <c r="B30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="3">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>169</v>
+      </c>
+      <c r="C31" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>213</v>
+      </c>
+      <c r="B32" t="s">
+        <v>113</v>
+      </c>
+      <c r="C32" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
+        <v>164</v>
+      </c>
+      <c r="C33" s="3">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>214</v>
+      </c>
+      <c r="B34" t="s">
+        <v>166</v>
+      </c>
+      <c r="C34" s="3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="3">
+        <v>500000</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B35">
+    <sortCondition ref="A2:A35"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE76A5D-7100-4896-AEFF-4E3A2F402CED}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C52412B7-2386-4655-B84B-EEB748633C00}">
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I2" sqref="I2:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.36328125" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2" s="5">
+        <v>45402</v>
+      </c>
+      <c r="I2" s="5">
+        <v>45395</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3">
+        <v>21</v>
+      </c>
+      <c r="H3" s="5">
+        <v>45403</v>
+      </c>
+      <c r="I3" s="5">
+        <v>45396</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>187</v>
+      </c>
+      <c r="G4">
+        <v>35</v>
+      </c>
+      <c r="H4" s="5">
+        <v>45404</v>
+      </c>
+      <c r="I4" s="5">
+        <v>45397</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5">
         <v>14</v>
       </c>
+      <c r="H5" s="5">
+        <v>45405</v>
+      </c>
+      <c r="I5" s="5">
+        <v>45398</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>189</v>
+      </c>
+      <c r="G6">
+        <v>40</v>
+      </c>
+      <c r="H6" s="5">
+        <v>45406</v>
+      </c>
+      <c r="I6" s="5">
+        <v>45399</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF1C386-722F-4295-863A-69DD06659867}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE76A5D-7100-4896-AEFF-4E3A2F402CED}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>183</v>
+      </c>
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create users, roles and privileges.
</commit_message>
<xml_diff>
--- a/Schema_Data/Data.xlsx
+++ b/Schema_Data/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Year3\HK2\PTTK\Project\Schema_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4CBFA5-C017-438D-8528-7E65A5438620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC2E4D6-F6B9-4669-9105-DD5C3005DC14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="10" activeTab="15" xr2:uid="{A9C2B380-941E-4AF3-AF89-697926482C6B}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{A9C2B380-941E-4AF3-AF89-697926482C6B}"/>
   </bookViews>
   <sheets>
     <sheet name="UNGVIEN" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="233">
   <si>
     <t>HOTEN</t>
   </si>
@@ -735,6 +735,21 @@
   </si>
   <si>
     <t>Overall 9.0</t>
+  </si>
+  <si>
+    <t>dn_vmquynh21@clc.fitus.edu.vn</t>
+  </si>
+  <si>
+    <t>dn_vdvthinh21@clc.fitus.edu.vn</t>
+  </si>
+  <si>
+    <t>dn_tvphuc21@clc.fitus.edu.vn</t>
+  </si>
+  <si>
+    <t>dn_nlhkha21@clc.fitus.edu.vn</t>
+  </si>
+  <si>
+    <t>dn_lttien21@clc.fitus.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -2744,7 +2759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB20A08-185D-48E3-8DB2-CDE84B0FEB50}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -2912,8 +2927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF92A007-D918-48FF-9D99-3B2B9E34C6B8}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2924,7 +2939,7 @@
     <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.54296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2974,7 +2989,7 @@
         <v>87</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>62</v>
+        <v>228</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -3000,7 +3015,7 @@
         <v>88</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>63</v>
+        <v>229</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -3026,7 +3041,7 @@
         <v>89</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>64</v>
+        <v>230</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -3052,7 +3067,7 @@
         <v>90</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>65</v>
+        <v>231</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -3078,7 +3093,7 @@
         <v>91</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="H6">
         <v>1</v>

</xml_diff>